<commit_message>
bug with editing subject fixed
</commit_message>
<xml_diff>
--- a/subjects.xlsx
+++ b/subjects.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\SubjectAkinator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
   </bookViews>
@@ -205,8 +210,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,12 +561,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -735,7 +734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -753,27 +752,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -801,6 +799,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -847,7 +853,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -879,9 +885,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -913,6 +920,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1088,14 +1096,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="56" customWidth="1"/>
     <col min="2" max="3" width="4.88671875" customWidth="1"/>
@@ -1110,7 +1118,7 @@
     <col min="14" max="15" width="4.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1136,7 @@
       </c>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1221,14 +1229,14 @@
       <c r="N3" s="3">
         <v>1</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="3">
         <v>4</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1271,14 +1279,14 @@
       <c r="N4" s="3">
         <v>1</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="3">
         <v>4</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1305,7 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>2</v>
       </c>
       <c r="H5" s="7" t="s">
@@ -1309,7 +1317,7 @@
       <c r="J5" s="1">
         <v>2</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>3</v>
       </c>
       <c r="L5" s="7" t="s">
@@ -1321,14 +1329,14 @@
       <c r="N5" s="3">
         <v>1</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="3">
         <v>4</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1347,7 +1355,7 @@
       <c r="F6" s="1">
         <v>2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>2</v>
       </c>
       <c r="H6" s="7" t="s">
@@ -1359,7 +1367,7 @@
       <c r="J6" s="1">
         <v>2</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>3</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -1371,14 +1379,14 @@
       <c r="N6" s="3">
         <v>1</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="3">
         <v>4</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1397,7 +1405,7 @@
       <c r="F7" s="1">
         <v>2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>2</v>
       </c>
       <c r="H7" s="7" t="s">
@@ -1409,7 +1417,7 @@
       <c r="J7" s="1">
         <v>2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>3</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -1421,14 +1429,14 @@
       <c r="N7" s="3">
         <v>1</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="3">
         <v>4</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1447,7 +1455,7 @@
       <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="3">
         <v>2</v>
       </c>
       <c r="H8" s="8" t="s">
@@ -1459,7 +1467,7 @@
       <c r="J8" s="1">
         <v>2</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>3</v>
       </c>
       <c r="L8" s="7" t="s">
@@ -1471,14 +1479,14 @@
       <c r="N8" s="3">
         <v>1</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="3">
         <v>4</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1497,7 +1505,7 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="3">
         <v>2</v>
       </c>
       <c r="H9" s="8" t="s">
@@ -1509,7 +1517,7 @@
       <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>3</v>
       </c>
       <c r="L9" s="7" t="s">
@@ -1521,14 +1529,14 @@
       <c r="N9" s="3">
         <v>1</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="3">
         <v>4</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1547,7 +1555,7 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="3">
         <v>2</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -1559,7 +1567,7 @@
       <c r="J10" s="3">
         <v>1</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="3">
         <v>3</v>
       </c>
       <c r="L10" s="8" t="s">
@@ -1571,14 +1579,14 @@
       <c r="N10" s="3">
         <v>1</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="3">
         <v>4</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1597,7 +1605,7 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="3">
         <v>2</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -1609,7 +1617,7 @@
       <c r="J11" s="3">
         <v>1</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="3">
         <v>3</v>
       </c>
       <c r="L11" s="8" t="s">
@@ -1621,14 +1629,14 @@
       <c r="N11" s="3">
         <v>1</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="3">
         <v>4</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1647,7 +1655,7 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="3">
         <v>2</v>
       </c>
       <c r="H12" s="8" t="s">
@@ -1659,7 +1667,7 @@
       <c r="J12" s="3">
         <v>1</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="3">
         <v>3</v>
       </c>
       <c r="L12" s="8" t="s">
@@ -1671,21 +1679,21 @@
       <c r="N12" s="3">
         <v>1</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="3">
         <v>4</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="3">
         <v>1</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -1697,7 +1705,7 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="3">
         <v>2</v>
       </c>
       <c r="H13" s="8" t="s">
@@ -1709,7 +1717,7 @@
       <c r="J13" s="3">
         <v>1</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="3">
         <v>3</v>
       </c>
       <c r="L13" s="8" t="s">
@@ -1717,14 +1725,14 @@
       </c>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -1736,7 +1744,7 @@
       <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="3">
         <v>2</v>
       </c>
       <c r="H14" s="8" t="s">
@@ -1748,7 +1756,7 @@
       <c r="J14" s="3">
         <v>1</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="3">
         <v>3</v>
       </c>
       <c r="L14" s="8" t="s">
@@ -1756,14 +1764,14 @@
       </c>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
@@ -1775,7 +1783,7 @@
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="3">
         <v>2</v>
       </c>
       <c r="H15" s="8" t="s">
@@ -1787,7 +1795,7 @@
       <c r="J15" s="3">
         <v>1</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="3">
         <v>3</v>
       </c>
       <c r="L15" s="8" t="s">
@@ -1795,14 +1803,14 @@
       </c>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="3">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -1815,7 +1823,7 @@
       <c r="J16" s="3">
         <v>1</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="3">
         <v>3</v>
       </c>
       <c r="L16" s="8" t="s">
@@ -1823,14 +1831,14 @@
       </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
       <c r="D17" s="8" t="s">
@@ -1843,7 +1851,7 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="3">
         <v>3</v>
       </c>
       <c r="L17" s="8" t="s">
@@ -1851,85 +1859,85 @@
       </c>
       <c r="P17" s="4"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>

</xml_diff>